<commit_message>
Updated stock bot documentation
</commit_message>
<xml_diff>
--- a/WrittenWorks/Documentation/StockBotDocumentation/StockBotGraphs.xlsx
+++ b/WrittenWorks/Documentation/StockBotDocumentation/StockBotGraphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arcti\IdeaProjects\ProbStatsProject2\WrittenWorks\Documentation\StockBotDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E35109-30C2-4401-96FD-F825D3AD60F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE45F8C-9AC7-449F-99BE-33B6D52A5525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A0CA121E-A588-43B5-9527-D026446EA530}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Seventy</t>
+  </si>
+  <si>
+    <t>Smoothed Close</t>
   </si>
 </sst>
 </file>
@@ -1744,6 +1747,805 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Smoothed Closing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Stock Values</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NintendoStockGraphs!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Close</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>NintendoStockGraphs!$E$2:$E$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>10.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.84</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.95</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.74</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.38</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.77</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.68</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.62</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.37</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.35</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10.47</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10.220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.07</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.23</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11.53</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.48</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11.73</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.79</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.79</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>12.17</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12.99</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12.49</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13.93</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13.74</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14.29</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14.58</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>13.96</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14.04</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>13.77</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>13.77</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>13.84</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>13.59</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>12.77</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12.41</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>12.22</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CDB3-4318-A6C8-8F2D0F7B24DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>NintendoStockGraphs!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Smoothed Close</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>NintendoStockGraphs!$K$2:$K$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>10.48666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.526666669999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.48666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.69333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.733333330000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.786666670000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.823333330000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.88666667</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.03</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.08333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.29666667</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.29666667</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.35333333</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.92333333</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.64666667</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.52333333</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.516666669999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10.626666670000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.596666669999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10.446666670000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10.39666667</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10.346666669999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10.25333333</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10.17333333</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10.366666670000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.81</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11.24333333</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.47</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11.58</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>11.66666667</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.77</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>11.91666667</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>12.31666667</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>12.55</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>13.13666667</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13.38666667</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>13.69</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13.81</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>14.09</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>14.39</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>14.28</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>13.92333333</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>13.86</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>13.793333329999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>13.733333330000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12.92333333</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>12.46666667</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>12.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CDB3-4318-A6C8-8F2D0F7B24DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1478573375"/>
+        <c:axId val="251874287"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1478573375"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Increment</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="251874287"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="251874287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Closing Price</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1478573375"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1824,6 +2626,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2856,20 +3698,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>530225</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>225425</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>174625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2896,16 +4254,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>530225</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>155575</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>606425</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>225425</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>301625</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2925,6 +4283,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98EBC076-E012-1E1A-4E5A-9A039BBCD490}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3250,10 +4644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F42C794-EC7D-4383-97C6-C93890A15EB4}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="D42" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3262,9 +4656,10 @@
     <col min="2" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3295,8 +4690,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45033</v>
       </c>
@@ -3327,8 +4725,11 @@
       <c r="J2">
         <v>70</v>
       </c>
+      <c r="K2">
+        <v>10.48666667</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45040</v>
       </c>
@@ -3356,8 +4757,11 @@
       <c r="J3">
         <v>70</v>
       </c>
+      <c r="K3">
+        <v>10.526666669999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45047</v>
       </c>
@@ -3385,8 +4789,11 @@
       <c r="J4">
         <v>70</v>
       </c>
+      <c r="K4">
+        <v>10.48666667</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45054</v>
       </c>
@@ -3414,8 +4821,11 @@
       <c r="J5">
         <v>70</v>
       </c>
+      <c r="K5">
+        <v>10.6</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45061</v>
       </c>
@@ -3443,8 +4853,11 @@
       <c r="J6">
         <v>70</v>
       </c>
+      <c r="K6">
+        <v>10.69333333</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45068</v>
       </c>
@@ -3472,8 +4885,11 @@
       <c r="J7">
         <v>70</v>
       </c>
+      <c r="K7">
+        <v>10.733333330000001</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45075</v>
       </c>
@@ -3501,8 +4917,11 @@
       <c r="J8">
         <v>70</v>
       </c>
+      <c r="K8">
+        <v>10.786666670000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45082</v>
       </c>
@@ -3530,8 +4949,11 @@
       <c r="J9">
         <v>70</v>
       </c>
+      <c r="K9">
+        <v>10.823333330000001</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45089</v>
       </c>
@@ -3559,8 +4981,11 @@
       <c r="J10">
         <v>70</v>
       </c>
+      <c r="K10">
+        <v>10.92</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45096</v>
       </c>
@@ -3588,8 +5013,11 @@
       <c r="J11">
         <v>70</v>
       </c>
+      <c r="K11">
+        <v>10.88666667</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>45103</v>
       </c>
@@ -3617,8 +5045,11 @@
       <c r="J12">
         <v>70</v>
       </c>
+      <c r="K12">
+        <v>11.03</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>45110</v>
       </c>
@@ -3646,8 +5077,11 @@
       <c r="J13">
         <v>70</v>
       </c>
+      <c r="K13">
+        <v>11.08333333</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>45117</v>
       </c>
@@ -3675,8 +5109,11 @@
       <c r="J14">
         <v>70</v>
       </c>
+      <c r="K14">
+        <v>11.29666667</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>45124</v>
       </c>
@@ -3704,8 +5141,11 @@
       <c r="J15">
         <v>70</v>
       </c>
+      <c r="K15">
+        <v>11.29666667</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>45131</v>
       </c>
@@ -3733,8 +5173,11 @@
       <c r="J16">
         <v>70</v>
       </c>
+      <c r="K16">
+        <v>11.35333333</v>
+      </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>45138</v>
       </c>
@@ -3762,8 +5205,11 @@
       <c r="J17">
         <v>70</v>
       </c>
+      <c r="K17">
+        <v>11.15</v>
+      </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>45145</v>
       </c>
@@ -3791,8 +5237,11 @@
       <c r="J18">
         <v>70</v>
       </c>
+      <c r="K18">
+        <v>10.92333333</v>
+      </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>45152</v>
       </c>
@@ -3820,8 +5269,11 @@
       <c r="J19">
         <v>70</v>
       </c>
+      <c r="K19">
+        <v>10.64666667</v>
+      </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>45159</v>
       </c>
@@ -3849,8 +5301,11 @@
       <c r="J20">
         <v>70</v>
       </c>
+      <c r="K20">
+        <v>10.52333333</v>
+      </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>45166</v>
       </c>
@@ -3878,8 +5333,11 @@
       <c r="J21">
         <v>70</v>
       </c>
+      <c r="K21">
+        <v>10.516666669999999</v>
+      </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>45173</v>
       </c>
@@ -3907,8 +5365,11 @@
       <c r="J22">
         <v>70</v>
       </c>
+      <c r="K22">
+        <v>10.626666670000001</v>
+      </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>45180</v>
       </c>
@@ -3936,8 +5397,11 @@
       <c r="J23">
         <v>70</v>
       </c>
+      <c r="K23">
+        <v>10.7</v>
+      </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>45187</v>
       </c>
@@ -3965,8 +5429,11 @@
       <c r="J24">
         <v>70</v>
       </c>
+      <c r="K24">
+        <v>10.596666669999999</v>
+      </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>45194</v>
       </c>
@@ -3994,8 +5461,11 @@
       <c r="J25">
         <v>70</v>
       </c>
+      <c r="K25">
+        <v>10.446666670000001</v>
+      </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>45201</v>
       </c>
@@ -4023,8 +5493,11 @@
       <c r="J26">
         <v>70</v>
       </c>
+      <c r="K26">
+        <v>10.39666667</v>
+      </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>45208</v>
       </c>
@@ -4052,8 +5525,11 @@
       <c r="J27">
         <v>70</v>
       </c>
+      <c r="K27">
+        <v>10.346666669999999</v>
+      </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>45215</v>
       </c>
@@ -4081,8 +5557,11 @@
       <c r="J28">
         <v>70</v>
       </c>
+      <c r="K28">
+        <v>10.25333333</v>
+      </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>45222</v>
       </c>
@@ -4110,8 +5589,11 @@
       <c r="J29">
         <v>70</v>
       </c>
+      <c r="K29">
+        <v>10.17333333</v>
+      </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>45229</v>
       </c>
@@ -4139,8 +5621,11 @@
       <c r="J30">
         <v>70</v>
       </c>
+      <c r="K30">
+        <v>10.366666670000001</v>
+      </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>45236</v>
       </c>
@@ -4168,8 +5653,11 @@
       <c r="J31">
         <v>70</v>
       </c>
+      <c r="K31">
+        <v>10.81</v>
+      </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>45243</v>
       </c>
@@ -4197,8 +5685,11 @@
       <c r="J32">
         <v>70</v>
       </c>
+      <c r="K32">
+        <v>11.24333333</v>
+      </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>45250</v>
       </c>
@@ -4226,8 +5717,11 @@
       <c r="J33">
         <v>70</v>
       </c>
+      <c r="K33">
+        <v>11.47</v>
+      </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>45257</v>
       </c>
@@ -4255,8 +5749,11 @@
       <c r="J34">
         <v>70</v>
       </c>
+      <c r="K34">
+        <v>11.58</v>
+      </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>45264</v>
       </c>
@@ -4284,8 +5781,11 @@
       <c r="J35">
         <v>70</v>
       </c>
+      <c r="K35">
+        <v>11.66666667</v>
+      </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>45271</v>
       </c>
@@ -4313,8 +5813,11 @@
       <c r="J36">
         <v>70</v>
       </c>
+      <c r="K36">
+        <v>11.77</v>
+      </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>45278</v>
       </c>
@@ -4342,8 +5845,11 @@
       <c r="J37">
         <v>70</v>
       </c>
+      <c r="K37">
+        <v>11.91666667</v>
+      </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>45285</v>
       </c>
@@ -4371,8 +5877,11 @@
       <c r="J38">
         <v>70</v>
       </c>
+      <c r="K38">
+        <v>12.31666667</v>
+      </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>45292</v>
       </c>
@@ -4400,8 +5909,11 @@
       <c r="J39">
         <v>70</v>
       </c>
+      <c r="K39">
+        <v>12.55</v>
+      </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>45299</v>
       </c>
@@ -4429,8 +5941,11 @@
       <c r="J40">
         <v>70</v>
       </c>
+      <c r="K40">
+        <v>13.13666667</v>
+      </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>45306</v>
       </c>
@@ -4458,8 +5973,11 @@
       <c r="J41">
         <v>70</v>
       </c>
+      <c r="K41">
+        <v>13.38666667</v>
+      </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>45313</v>
       </c>
@@ -4487,8 +6005,11 @@
       <c r="J42">
         <v>70</v>
       </c>
+      <c r="K42">
+        <v>13.69</v>
+      </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>45320</v>
       </c>
@@ -4516,8 +6037,11 @@
       <c r="J43">
         <v>70</v>
       </c>
+      <c r="K43">
+        <v>13.81</v>
+      </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>45327</v>
       </c>
@@ -4545,8 +6069,11 @@
       <c r="J44">
         <v>70</v>
       </c>
+      <c r="K44">
+        <v>14.09</v>
+      </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>45334</v>
       </c>
@@ -4574,8 +6101,11 @@
       <c r="J45">
         <v>70</v>
       </c>
+      <c r="K45">
+        <v>14.39</v>
+      </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45341</v>
       </c>
@@ -4603,8 +6133,11 @@
       <c r="J46">
         <v>70</v>
       </c>
+      <c r="K46">
+        <v>14.28</v>
+      </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45348</v>
       </c>
@@ -4632,8 +6165,11 @@
       <c r="J47">
         <v>70</v>
       </c>
+      <c r="K47">
+        <v>14.1</v>
+      </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>45355</v>
       </c>
@@ -4661,8 +6197,11 @@
       <c r="J48">
         <v>70</v>
       </c>
+      <c r="K48">
+        <v>13.92333333</v>
+      </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>45362</v>
       </c>
@@ -4690,8 +6229,11 @@
       <c r="J49">
         <v>70</v>
       </c>
+      <c r="K49">
+        <v>13.86</v>
+      </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>45369</v>
       </c>
@@ -4719,8 +6261,11 @@
       <c r="J50">
         <v>70</v>
       </c>
+      <c r="K50">
+        <v>13.793333329999999</v>
+      </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>45376</v>
       </c>
@@ -4748,8 +6293,11 @@
       <c r="J51">
         <v>70</v>
       </c>
+      <c r="K51">
+        <v>13.733333330000001</v>
+      </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>45383</v>
       </c>
@@ -4777,8 +6325,11 @@
       <c r="J52">
         <v>70</v>
       </c>
+      <c r="K52">
+        <v>13.4</v>
+      </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>45390</v>
       </c>
@@ -4806,8 +6357,11 @@
       <c r="J53">
         <v>70</v>
       </c>
+      <c r="K53">
+        <v>12.92333333</v>
+      </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>45397</v>
       </c>
@@ -4835,8 +6389,11 @@
       <c r="J54">
         <v>70</v>
       </c>
+      <c r="K54">
+        <v>12.46666667</v>
+      </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>45400</v>
       </c>
@@ -4863,6 +6420,9 @@
       </c>
       <c r="J55">
         <v>70</v>
+      </c>
+      <c r="K55">
+        <v>12.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>